<commit_message>
Revert "add new level"
This reverts commit 855ab3f358c7ca8d5e404a5069fe60fa2a04296d.
</commit_message>
<xml_diff>
--- a/BlockDisappear/docments/levels-difficult.xlsx
+++ b/BlockDisappear/docments/levels-difficult.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="14600" yWindow="540" windowWidth="33600" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,16 +217,6 @@
   </si>
   <si>
     <t>Level-ct4a-5-1125</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Level-ct4a-4-1201</t>
-  </si>
-  <si>
-    <t>Level-ct4a-4-1201-2</t>
-  </si>
-  <si>
-    <t>难关</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -292,12 +282,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -342,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="39">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
@@ -363,8 +349,6 @@
     <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -384,8 +368,6 @@
     <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -660,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1069,7 +1051,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1083,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1100,7 +1082,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -1114,8 +1096,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B37">
@@ -1131,8 +1113,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B38">
@@ -1146,43 +1128,6 @@
       </c>
       <c r="E38" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "add new level""
This reverts commit 323790a5321d7691e4b65ddc1869b2d721dfdda5.
</commit_message>
<xml_diff>
--- a/BlockDisappear/docments/levels-difficult.xlsx
+++ b/BlockDisappear/docments/levels-difficult.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="540" windowWidth="33600" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,6 +217,16 @@
   </si>
   <si>
     <t>Level-ct4a-5-1125</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level-ct4a-4-1201</t>
+  </si>
+  <si>
+    <t>Level-ct4a-4-1201-2</t>
+  </si>
+  <si>
+    <t>难关</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -282,8 +292,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -328,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="43">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
@@ -349,6 +363,8 @@
     <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -368,6 +384,8 @@
     <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1034,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1051,7 +1069,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1100,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -1096,8 +1114,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B37">
@@ -1113,8 +1131,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B38">
@@ -1128,6 +1146,43 @@
       </c>
       <c r="E38" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>